<commit_message>
Added landing page. Not linked yet but still cool.
</commit_message>
<xml_diff>
--- a/merged_data.xlsx
+++ b/merged_data.xlsx
@@ -436,228 +436,228 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>People</t>
+          <t>Brand</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Brand</t>
+          <t>Customer</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>peoplefile1</t>
+          <t>brandfile1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>peoplefile2</t>
+          <t>brandfile2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to landing page design. Minor adjustments to other functionality as well.
</commit_message>
<xml_diff>
--- a/merged_data.xlsx
+++ b/merged_data.xlsx
@@ -436,228 +436,228 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Brand</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Customer</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>brandfile1</t>
+          <t>customerfiel1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>customerfiel1</t>
+          <t>brandfile1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>brandfile2</t>
+          <t>customerfiel2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>customerfiel2</t>
+          <t>brandfile2</t>
         </is>
       </c>
     </row>

</xml_diff>